<commit_message>
[Experiments] Adding 2 columns for description and query number.
</commit_message>
<xml_diff>
--- a/experiment_1/queries.xlsx
+++ b/experiment_1/queries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadine/Desktop/Thesis/BA_Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadine/Desktop/BA_Thesis/experiment_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70715DBD-4843-1245-AE42-B30C33F7C719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF37950-4F15-1F46-BD6C-2825323888B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17360" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Type</t>
   </si>
@@ -134,6 +134,48 @@
     <t>MATCH (w:ifc__IfcWindow)&lt;--(:ifc__IfcRelFillsElement)--&gt;(:ifc__IfcOpeningElement)
 			&lt;--(:ifc__IfcRelVoidsElement)--&gt;(wall:ifc__IfcWall) 
 RETURN DISTINCT wall</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Retrieve all components of the building which are generic placeholder</t>
+  </si>
+  <si>
+    <t>Retrieve all walls with a window</t>
+  </si>
+  <si>
+    <t>Retrieve  all walls with a door</t>
+  </si>
+  <si>
+    <t>Query all doors, windows, walls and slabs</t>
+  </si>
+  <si>
+    <t>Query the name of the construction project</t>
+  </si>
+  <si>
+    <t>Retrieve the wall with the name Basiswand:STB 250</t>
+  </si>
+  <si>
+    <t>Query doors with reference DL - 900 x 2175</t>
+  </si>
+  <si>
+    <t>Query number of doors that are not the entry door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrieve the highest door </t>
+  </si>
+  <si>
+    <t>Retrieve a wall in which a window with the smallest width is embedded</t>
+  </si>
+  <si>
+    <t>Query all walls that connections at least two rooms → these are walls that have at least 2 doors</t>
+  </si>
+  <si>
+    <t>Retrieve the number of rooms</t>
+  </si>
+  <si>
+    <t>Query Number</t>
   </si>
 </sst>
 </file>
@@ -488,158 +530,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF80A08-7EAB-A54A-9D47-86295BB267AC}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="103.83203125" customWidth="1"/>
-    <col min="3" max="3" width="118.33203125" customWidth="1"/>
+    <col min="2" max="2" width="73.6640625" customWidth="1"/>
+    <col min="4" max="4" width="103.83203125" customWidth="1"/>
+    <col min="5" max="5" width="131.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Experiments] Changes in the queries
</commit_message>
<xml_diff>
--- a/experiment_1/queries.xlsx
+++ b/experiment_1/queries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadine/Desktop/BA_Thesis/experiment_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadine/Desktop/BA/BA_Thesis/experiment_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF37950-4F15-1F46-BD6C-2825323888B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3ACCE3-815E-BA48-A56B-1B84D2DD0EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17360" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_1" sheetId="1" r:id="rId1"/>
@@ -36,68 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>MATCH (e{Entity:"IfcSpace"}) RETURN e</t>
-  </si>
-  <si>
-    <t>MATCH (e:ifc__IfcSpaceType) RETURN e</t>
-  </si>
-  <si>
-    <t>MATCH (n)--&gt;(m)--&gt;(o) 
-WHERE (n.Entity="IfcWall" AND m.Entity="IfcOpeningElement") AND o.Entity="IfcWindow" 
-RETURN DISTINCT n</t>
-  </si>
-  <si>
-    <t>MATCH (w{Entity:"IfcWall"})--&gt;({Entity:"IfcOpeningElement"})--&gt;(d{Entity:"IfcDoor"}) RETURN DISTINCT w</t>
-  </si>
-  <si>
-    <t>MATCH (d:ifc__IfcDoor)&lt;--(:ifc__IfcRelFillsElement)--&gt;(:ifc__IfcOpeningElement)&lt;--(:ifc__IfcRelVoidsElement)--&gt;(w:ifc__IfcWall) RETURN DISTINCT w</t>
-  </si>
-  <si>
-    <t>MATCH (e) WHERE e.Entity IN ["IfcSlab", "IfcWall", "IfcDoor", "IfcStair", "IfcWindow"] RETURN e</t>
-  </si>
-  <si>
     <t>MATCH (e) WHERE ANY (x IN labels(e) WHERE x IN ["ifc__IfcSlab", "ifc__IfcWall", "ifc__IfcDoor", "ifc__IfcStair", "ifc__IfcWindow"]) RETURN e</t>
-  </si>
-  <si>
-    <t>MATCH (p{Entity:"IfcProject"}) RETURN p.Name</t>
-  </si>
-  <si>
-    <t>MATCH (p:ifc__IfcProject)-[:ifc__name_IfcRoot]-&gt;(id:ifc__IfcLabel) 
-RETURN DISTINCT id.express__hasString[0]</t>
-  </si>
-  <si>
-    <t>MATCH (w{Entity:"IfcWall"}) WHERE w.Name CONTAINS "Basiswand:STB 250" RETURN w</t>
-  </si>
-  <si>
-    <t>MATCH (d{Entity:"IfcDoor"}) 
-WHERE d.Name CONTAINS "DL - 900 x 2175:2503001" 
-RETURN d</t>
-  </si>
-  <si>
-    <t>MATCH (d{Entity:"IfcDoor"}) WHERE NOT (d.Name CONTAINS "Haustür") RETURN COUNT (d) AS NumberDoors</t>
-  </si>
-  <si>
-    <t>MATCH (d{Entity:"IfcDoor"}) &lt;--(e) RETURN d ORDER BY e.Height DESC LIMIT 1</t>
-  </si>
-  <si>
-    <t>MATCH (d:ifc__IfcDoor)-[:ifc__overallHeight_IfcDoor]-&gt;(e:ifc__IfcLengthMeasure) 
-RETURN d
-ORDER BY e.express__hasDouble[0] DESC 
-LIMIT 1</t>
-  </si>
-  <si>
-    <t>MATCH (w1{Entity:"IfcWall"})--&gt;({Entity:"IfcOpeningElement"})--&gt;(w2{Entity:"IfcWindow"}) RETURN w1 ORDER BY w2.Height ASC LIMIT 1</t>
-  </si>
-  <si>
-    <t>MATCH (e:ifc__IfcPositiveLengthMeasure) &lt;--(w:ifc__IfcWindow)&lt;--(:ifc__IfcRelFillsElement)--&gt;(:ifc__IfcOpeningElement)&lt;--(:ifc__IfcRelVoidsElement)--&gt;(wall:ifc__IfcWall)
-RETURN w
-ORDER BY e.express__hasDouble[0] ASC 
-LIMIT 1</t>
   </si>
   <si>
     <t>MATCH (d1{Entity:"IfcDoor"})&lt;--(r1{Entity:"IfcOpeningElement"})&lt;--(w{Entity:"IfcWall"}) --&gt; (r2{Entity:"IfcOpeningElement"})--&gt;(d2{Entity:"IfcDoor"}) 
@@ -108,74 +52,108 @@
     <t>MATCH (d1:ifc__IfcDoor)&lt;--(:ifc__IfcRelFillsElement)--&gt;(:ifc__IfcOpeningElement)&lt;--(:ifc__IfcRelVoidsElement)--&gt;(w:ifc__IfcWall) &lt;--(:ifc__IfcRelVoidsElement)--&gt;(:ifc__IfcOpeningElement)&lt;--(:ifc__IfcRelFillsElement)--&gt;(d2:ifc__IfcDoor) WHERE d1&lt;&gt;d2 RETURN DISTINCT w</t>
   </si>
   <si>
-    <t>Match (w1{Entity:"IfcWall"}) --&gt;(w2{Entity:"IfcWall"}) --&gt; (w3{Entity:"IfcWall"})&lt;-- (w4{Entity:"IfcWall"})--&gt;(w1) RETURN COUNT(w1) AS NumberRooms</t>
-  </si>
-  <si>
-    <t>MATCH (w1:ifc__IfcWall) &lt;-[:ifc__relatingElement_IfcRelConnectsElements]- (:ifc__IfcRelConnectsPathElements) -[:ifc__relatedElement_IfcRelConnectsElements]-&gt; (w2:ifc__IfcWall) &lt;-[:ifc__relatingElement_IfcRelConnectsElements]-( :ifc__IfcRelConnectsPathElements) -[:ifc__relatedElement_IfcRelConnectsElements]-&gt; (w3:ifc__IfcWall) &lt;-[:ifc__relatingElement_IfcRelConnectsElements]-( :ifc__IfcRelConnectsPathElements)-[:ifc__relatedElement_IfcRelConnectsElements]-&gt;(w4:ifc__IfcWall) &lt;-[:ifc__relatedElement_IfcRelConnectsElements]-(:ifc__IfcRelConnectsPathElements)-[:ifc__relatingElement_IfcRelConnectsElements]-&gt;(w1) RETURN COUNT(w1) AS NumberRooms</t>
-  </si>
-  <si>
     <t>LPG</t>
   </si>
   <si>
     <t>RDF</t>
   </si>
   <si>
-    <t>MATCH (w:ifc_IfcWall)--&gt;(l:ifc_IfcLabel) WHERE l.express_hasString CONTAINS "Basiswand:STB 250" RETURN w</t>
-  </si>
-  <si>
-    <t>MATCH (label:ifc__IfcLabel)&lt;--(d:ifc__IfcDoor) WHERE NOT (label.express__hasString[0] CONTAINS "Haust\X\FCre") RETURN DISTINCT d</t>
-  </si>
-  <si>
-    <t>MATCH (d:ifc__IfcDoor)--&gt;(l:ifc__IfcLabel)
-WHERE l.express__hasString[0] CONTAINS "DL - 900 x 2175:2503001"
-RETURN d</t>
-  </si>
-  <si>
-    <t>MATCH (w:ifc__IfcWindow)&lt;--(:ifc__IfcRelFillsElement)--&gt;(:ifc__IfcOpeningElement)
-			&lt;--(:ifc__IfcRelVoidsElement)--&gt;(wall:ifc__IfcWall) 
-RETURN DISTINCT wall</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve"> Retrieve all components of the building which are generic placeholder</t>
-  </si>
-  <si>
-    <t>Retrieve all walls with a window</t>
-  </si>
-  <si>
-    <t>Retrieve  all walls with a door</t>
-  </si>
-  <si>
-    <t>Query all doors, windows, walls and slabs</t>
-  </si>
-  <si>
-    <t>Query the name of the construction project</t>
-  </si>
-  <si>
     <t>Retrieve the wall with the name Basiswand:STB 250</t>
   </si>
   <si>
-    <t>Query doors with reference DL - 900 x 2175</t>
-  </si>
-  <si>
-    <t>Query number of doors that are not the entry door</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retrieve the highest door </t>
-  </si>
-  <si>
-    <t>Retrieve a wall in which a window with the smallest width is embedded</t>
-  </si>
-  <si>
-    <t>Query all walls that connections at least two rooms → these are walls that have at least 2 doors</t>
-  </si>
-  <si>
-    <t>Retrieve the number of rooms</t>
-  </si>
-  <si>
     <t>Query Number</t>
+  </si>
+  <si>
+    <t>MATCH (e{Entity:"IfcSpace"})
+RETURN Distinct e</t>
+  </si>
+  <si>
+    <t>MATCH (e:ifc__IfcSpace)
+RETURN e</t>
+  </si>
+  <si>
+    <t>MATCH (w{Entity:"IfcWall"})
+RETURN w</t>
+  </si>
+  <si>
+    <t>MATCH (w:ifc__IfcWall) RETURN w</t>
+  </si>
+  <si>
+    <t>MATCH (e)
+WHERE e.Entity IN ["IfcSlab", "IfcWall", "IfcDoor", "IfcStair", "IfcWindow"]
+RETURN e</t>
+  </si>
+  <si>
+    <t>MATCH (w{Entity:"IfcWall"}) 
+WHERE w.Name CONTAINS "Basiswand:STB 250"
+RETURN w</t>
+  </si>
+  <si>
+    <t>MATCH (w:ifc_IfcWall)--&gt;(l:ifc_IfcLabel)
+WHERE l.express_hasString[0] CONTAINS "Basiswand:STB 250"
+RETURN w</t>
+  </si>
+  <si>
+    <t>Query the width and height of all doors</t>
+  </si>
+  <si>
+    <t>MATCH (p{Entity:"IfcOpeningElement"})--&gt;({Entity:"IfcDoor"}) 
+WHERE NOT (p.Width = "null" OR p.Height = "null")
+RETURN p.Width As Width, p.Height AS Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (e1:ifc__IfcPositiveLengthMeasure)&lt;-[:ifc__overallWidth_IfcDoor]-(:ifc__IfcDoor)-[:ifc__overallHeight_IfcDoor]-&gt;(e2:ifc__IfcPositiveLengthMeasure)
+RETURN e1.express__hasDouble[0] AS Width, e2.express__hasDouble[0] AS Height  </t>
+  </si>
+  <si>
+    <t>MATCH (d{Entity:"IfcDoor"})
+WHERE NOT (d.Name CONTAINS "Haustür")
+RETURN COUNT (d) AS NumberDoors</t>
+  </si>
+  <si>
+    <t>MATCH (label:ifc__IfcLabel)&lt;-- (d:ifc__IfcDoor) 
+WHERE NOT (label.express__hasString[0] CONTAINS "Haust\X\FCre")
+RETURN DISTINCT d</t>
+  </si>
+  <si>
+    <t>MATCH (w{Entity:"IfcWall"})--&gt;(e{Entity:"IfcOpeningElement"})--&gt;({Entity:"IfcWindow"}) RETURN DISTINCT w</t>
+  </si>
+  <si>
+    <t>Retrieve all walls in which a window is embedded</t>
+  </si>
+  <si>
+    <t>MATCH (:ifc__IfcWindow)&lt;--(:ifc__IfcRelFillsElement)--&gt;(:ifc__IfcOpeningElement)&lt;--(:ifc__IfcRelVoidsElement)--&gt;(w:ifc__IfcWall) RETURN DISTINCT w</t>
+  </si>
+  <si>
+    <t>Query all walls that have at least 2 doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrieve the number of rooms created by 4 walls </t>
+  </si>
+  <si>
+    <t>Match (w1{Entity:"IfcWall"}) --&gt;(w2{Entity:"IfcWall"}) --&gt; (w3{Entity:"IfcWall"})&lt;-- (w4{Entity:"IfcWall"})--&gt;(w1)  
+RETURN COUNT(w1) AS NumberRooms</t>
+  </si>
+  <si>
+    <t>MATCH (w1:ifc__IfcWall) &lt;-[:ifc__relatingElement_IfcRelConnectsElements]- (:ifc__IfcRelConnectsPathElements) -[:ifc__relatedElement_IfcRelConnectsElements]-&gt; (w2:ifc__IfcWall) 
+				&lt;-[:ifc__relatingElement_IfcRelConnectsElements]-( :ifc__IfcRelConnectsPathElements) -[:ifc__relatedElement_IfcRelConnectsElements]-&gt; (w3:ifc__IfcWall) 
+				&lt;-[:ifc__relatingElement_IfcRelConnectsElements]-( :ifc__IfcRelConnectsPathElements)-[:ifc__relatedElement_IfcRelConnectsElements]-&gt;(w4:ifc__IfcWall) &lt;-[:ifc__relatedElement_IfcRelConnectsElements]-(:ifc__IfcRelConnectsPathElements)-[:ifc__relatingElement_IfcRelConnectsElements]-&gt;(w1)
+RETURN COUNT(w1) AS NumberRooms</t>
+  </si>
+  <si>
+    <t>Retrieve all components of the building which are generic placeholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrieve all walls </t>
+  </si>
+  <si>
+    <t>Retrieve all doors, windows, walls and slabs</t>
+  </si>
+  <si>
+    <t>Retrieve number of doors that are not the entry door “Haustür”</t>
   </si>
 </sst>
 </file>
@@ -530,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF80A08-7EAB-A54A-9D47-86295BB267AC}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,22 +523,22 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -570,14 +548,14 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -588,13 +566,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -604,164 +582,113 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
       <c r="E9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>13</v>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>